<commit_message>
add script to launch batches and version upgrade
</commit_message>
<xml_diff>
--- a/dvdtheque-batch/src/test/resources/export.xlsx
+++ b/dvdtheque-batch/src/test/resources/export.xlsx
@@ -88,6 +88,249 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>DAVID LYNCH</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>BLUE VELVET</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>1986</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>LAURA DERN,KYLE MACLACHLAN,HOPE LANGE,ISABELLA ROSSELLINI,GEORGE DICKERSON,DENNIS HOPPER,DEAN STOCKWELL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DAVID LYNCH</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>ERASERHEAD</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>1977</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>JEANNE BATES,JUDITH ROBERTS,LAUREL NEAR,JACK NANCE,CHARLOTTE STEWART,ALLEN JOSEPH,T. MAX GRAHAM</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DAVID LYNCH</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>LOST HIGHWAY</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>1997</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>BILL PULLMAN,PATRICIA ARQUETTE,ROBERT BLAKE,BALTHAZAR GETTY,LOUIS EPPOLITO,JOHN ROSELIUS,JENNA MAETLIND</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>DAVID LYNCH</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>MULHOLLAND DRIVE</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>2001</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>ROBERT FORSTER,LAURA HARRING,NAOMI WATTS,ANN MILLER,BRENT BRISCOE,JUSTIN THEROUX,DAN HEDAYA</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>MARTIN SCORSESE</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>RAGING BULL</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>1980</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>ROBERT DE NIRO,JOE PESCI,FRANK VINCENT,MARIO GALLO,CATHY MORIARTY,NICHOLAS COLASANTO,THERESA SALDANA</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>DAVID LYNCH</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>SAILOR ET LULA</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>1990</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>LAURA DERN,CRISPIN GLOVER,NICOLAS CAGE,WILLEM DAFOE,J.E. FREEMAN,CALVIN LOCKHART,DIANE LADD</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MARTIN SCORSESE</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>TAXI DRIVER</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>1976</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>ROBERT DE NIRO,CYBILL SHEPHERD,HARVEY KEITEL,JODIE FOSTER,ALBERT BROOKS,PETER BOYLE,LEONARD HARRIS</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DAVID LYNCH</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>TWIN PEAKS</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>1989</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>MÄDCHEN AMICK,KYLE MACLACHLAN,DANA ASHBROOK,SHERILYN FENN,LARA FLYNN BOYLE,MICHAEL ONTKEAN,RICHARD BEYMER</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DAVID LYNCH</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>UNE HISTOIRE VRAIE</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>1999</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>DONALD WIEGERT,TRACEY MALONEY,RICHARD FARNSWORTH,JANE GALLOWAY HEITZ,SISSY SPACEK,DAN FLANNERY,JOSEPH A. CARPENTER</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>